<commit_message>
# deliveryMap-GrupoLamas.xlsx en progreso
</commit_message>
<xml_diff>
--- a/docs/deliveryMap-GrupoLamas.xlsx
+++ b/docs/deliveryMap-GrupoLamas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Iteracion #1</t>
   </si>
@@ -43,22 +43,61 @@
     <t>Bloques</t>
   </si>
   <si>
-    <t>Spike Archivo Bloques RLV</t>
-  </si>
-  <si>
-    <t>Spike Archivo Bloques RLF</t>
-  </si>
-  <si>
     <t>Arbol B+</t>
   </si>
   <si>
     <t>Hash</t>
   </si>
   <si>
-    <t>Bloque RLF Árbol y Hash</t>
-  </si>
-  <si>
-    <t>CRUD Nodo Hoja</t>
+    <t>Estabilización</t>
+  </si>
+  <si>
+    <t>Documentación</t>
+  </si>
+  <si>
+    <t>Diagrama clases</t>
+  </si>
+  <si>
+    <t>Diagrama secuencias</t>
+  </si>
+  <si>
+    <t>Mapa entregables</t>
+  </si>
+  <si>
+    <t>Ejemplos de uso</t>
+  </si>
+  <si>
+    <t>Menu operaciones</t>
+  </si>
+  <si>
+    <t>Bug Fixes</t>
+  </si>
+  <si>
+    <t>Act doc organizacional</t>
+  </si>
+  <si>
+    <t>Archivos carga</t>
+  </si>
+  <si>
+    <t>Log-in</t>
+  </si>
+  <si>
+    <t>Aplicación</t>
+  </si>
+  <si>
+    <t>Automatización voto</t>
+  </si>
+  <si>
+    <t>Reportes</t>
+  </si>
+  <si>
+    <t>Actualizar</t>
+  </si>
+  <si>
+    <t>Obtener primero</t>
+  </si>
+  <si>
+    <t>Manejo bloques libres</t>
   </si>
 </sst>
 </file>
@@ -126,7 +165,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,12 +181,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -189,18 +222,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -244,30 +271,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="hair">
         <color indexed="64"/>
       </left>
@@ -286,31 +289,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -360,22 +339,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -392,86 +360,41 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -488,41 +411,71 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,8 +508,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>214288</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>373826</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>162159</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -604,8 +557,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>214288</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>350014</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>138347</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -653,8 +606,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>219051</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>361923</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>150256</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -683,6 +636,300 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2914650" y="971550"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>190476</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>10561</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10160000" y="839263"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1332442</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>178835</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>26428</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10148359" y="1278463"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>34929</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12659</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>225405</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>41207</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10194929" y="2626742"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1573745</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>16899</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>187304</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>24280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8569328" y="852982"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1066</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>10547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>191542</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>17928</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8573566" y="1058297"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>15887</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>4195</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>206363</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>11577</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8588387" y="1263612"/>
           <a:ext cx="190476" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -982,11 +1229,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T21"/>
+  <dimension ref="B2:T23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <selection pane="topRight" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,62 +1267,62 @@
     </row>
     <row r="3" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
-      <c r="C3" s="36">
+      <c r="C3" s="21">
         <v>40798</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37">
+      <c r="D3" s="21"/>
+      <c r="E3" s="22">
         <f>C3+7</f>
         <v>40805</v>
       </c>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22">
         <f t="shared" ref="G3" si="0">E3+7</f>
         <v>40812</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="35">
+      <c r="H3" s="22"/>
+      <c r="I3" s="20">
         <f>G3+7</f>
         <v>40819</v>
       </c>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35">
+      <c r="J3" s="20"/>
+      <c r="K3" s="20">
         <f>I3+7</f>
         <v>40826</v>
       </c>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35">
+      <c r="L3" s="20"/>
+      <c r="M3" s="20">
         <f>K3+7</f>
         <v>40833</v>
       </c>
-      <c r="N3" s="35"/>
+      <c r="N3" s="20"/>
     </row>
     <row r="4" spans="2:20" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="25"/>
-      <c r="C4" s="33" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="33" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="33" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="33" t="s">
+      <c r="H4" s="19"/>
+      <c r="I4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="34"/>
-      <c r="K4" s="33" t="s">
+      <c r="J4" s="19"/>
+      <c r="K4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="34"/>
-      <c r="M4" s="33" t="s">
+      <c r="L4" s="19"/>
+      <c r="M4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="34"/>
+      <c r="N4" s="19"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -1083,121 +1330,175 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="2:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+    <row r="5" spans="2:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="11" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="30"/>
+      <c r="N5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="22"/>
-    </row>
-    <row r="6" spans="2:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="49" t="s">
+    </row>
+    <row r="6" spans="2:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="35"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="31"/>
+      <c r="N6" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="22"/>
-    </row>
-    <row r="7" spans="2:20" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="41"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="30"/>
+    </row>
+    <row r="7" spans="2:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="35"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="37"/>
+      <c r="N7" s="36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="35"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="42" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="43" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="N10" s="32"/>
-    </row>
-    <row r="11" spans="2:20" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="M11" s="39"/>
+      <c r="N11" s="39" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="4"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="M15" s="38"/>
+      <c r="N15" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="44" t="s">
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="44"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C16" s="45" t="s">
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="45"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="46" t="s">
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="46"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B5:B8"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="M4:N4"/>
@@ -1210,6 +1511,13 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1218,6 +1526,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxKeywordTaxHTField xmlns="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <TaxCatchAll xmlns="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100334BCE8D889DEF4D8118EAEBC7DDD6B2" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a9e8cdd0e52f65fd6658b59d8085902">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89803a6daf5a3c19d83a5939325ddd43" ns2:_="">
     <xsd:import namespace="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84"/>
@@ -1369,27 +1697,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B9CCC97-E7A1-4F27-9745-AD74F7374CAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxKeywordTaxHTField xmlns="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <TaxCatchAll xmlns="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D643F50-9742-4664-BEE4-3C5D7337C66D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5B402D4-7882-4319-AA0E-83388EE1282B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1405,28 +1737,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D643F50-9742-4664-BEE4-3C5D7337C66D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B9CCC97-E7A1-4F27-9745-AD74F7374CAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
# Delivery map terminado
</commit_message>
<xml_diff>
--- a/docs/deliveryMap-GrupoLamas.xlsx
+++ b/docs/deliveryMap-GrupoLamas.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="405" windowWidth="14805" windowHeight="7710" tabRatio="736"/>
   </bookViews>
   <sheets>
-    <sheet name="Mapa Entregables" sheetId="12" r:id="rId1"/>
+    <sheet name="Mapa Entregables - Asignaciones" sheetId="12" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
   <si>
     <t>Iteracion #1</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Reportes</t>
   </si>
   <si>
-    <t>Actualizar</t>
-  </si>
-  <si>
     <t>Obtener primero</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
     <t>Bloque indice</t>
   </si>
   <si>
-    <t>Bloque archivo datos</t>
-  </si>
-  <si>
     <t>B, A</t>
   </si>
   <si>
@@ -269,6 +263,69 @@
   </si>
   <si>
     <t>Baja</t>
+  </si>
+  <si>
+    <t>Modificar</t>
+  </si>
+  <si>
+    <t>Separar raiz (int y hoja)</t>
+  </si>
+  <si>
+    <t>Disminuir altura</t>
+  </si>
+  <si>
+    <t>Bloque árbol</t>
+  </si>
+  <si>
+    <t>Bloque RLV</t>
+  </si>
+  <si>
+    <t>Bloque hash</t>
+  </si>
+  <si>
+    <t>Doc organizacional</t>
+  </si>
+  <si>
+    <t>Especificación clases</t>
+  </si>
+  <si>
+    <t>B, H, En</t>
+  </si>
+  <si>
+    <t>Nodo</t>
+  </si>
+  <si>
+    <t>Nodo interno</t>
+  </si>
+  <si>
+    <t>Archivo bloques RLV</t>
+  </si>
+  <si>
+    <t>ABM Nodo Hoja</t>
+  </si>
+  <si>
+    <t>Registro Variable</t>
+  </si>
+  <si>
+    <t>B, A, D, En</t>
+  </si>
+  <si>
+    <t>A, D, En</t>
+  </si>
+  <si>
+    <t>[Spike] Alta archivo RLF</t>
+  </si>
+  <si>
+    <t>[Spike] Baja archivo RLF</t>
+  </si>
+  <si>
+    <t>[Spike] Modif. archivo RLF</t>
+  </si>
+  <si>
+    <t>Miembro</t>
+  </si>
+  <si>
+    <t>Asignación tareas</t>
   </si>
 </sst>
 </file>
@@ -330,13 +387,13 @@
     </font>
     <font>
       <strike/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,12 +450,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -442,6 +505,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -452,6 +539,19 @@
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -527,11 +627,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -545,26 +678,41 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -581,56 +729,26 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -644,34 +762,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -683,31 +789,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -716,19 +810,127 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -754,153 +956,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>154778</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>214288</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>162159</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1219729" y="1202528"/>
-          <a:ext cx="190476" cy="219048"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>130966</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>214288</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>138347</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1214437" y="952497"/>
-          <a:ext cx="190476" cy="219048"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>219051</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>150256</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2914650" y="971550"/>
-          <a:ext cx="190476" cy="219048"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
@@ -953,13 +1008,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>9522</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>8463</xdr:rowOff>
+      <xdr:rowOff>209546</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>199998</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>15845</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>26428</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -987,7 +1042,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10455272" y="1267880"/>
+          <a:off x="10455272" y="1468963"/>
           <a:ext cx="190476" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1625,6 +1680,2113 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8613798" y="3215176"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>43399</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>233875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28547</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8806399" y="1661582"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>39216</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>16899</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>229692</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>24280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6833716" y="852982"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>43454</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>10547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>233930</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>17928</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6837954" y="1058297"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45568</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>236044</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>30618</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6840068" y="2806653"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>49806</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>16885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>240282</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45433</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6844306" y="3011968"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45568</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>236044</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>41225</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6840068" y="2055260"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>49806</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>16921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>240282</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>45469</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6844306" y="1869004"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>54044</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>10582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>244520</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>39130</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6848544" y="1481665"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>58282</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>4243</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>248758</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>11625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6852782" y="1263660"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28640</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>6326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219116</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>34874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6823140" y="2239409"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>32878</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>10558</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>223354</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>39106</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6827378" y="2434141"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>26533</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>14790</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>217009</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>43338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6821033" y="2628873"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>51937</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>242413</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47557</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6846437" y="3204592"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>54038</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>244514</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28547</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6848538" y="1661582"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1599265</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>232804</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>181074</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7352</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4911848" y="836054"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1603503</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>205286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>185312</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4916086" y="1041369"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1605617</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>175642</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>187426</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>13690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4918200" y="2789725"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>191664</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28505</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4922438" y="2995040"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1605617</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>186249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>187426</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>24297</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4918200" y="2038332"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190493</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>191664</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28541</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4922438" y="1852076"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5426</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>205320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>195902</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>22202</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4926676" y="1464737"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9664</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>198982</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200140</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>206363</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4930914" y="1246732"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1588689</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>179898</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>170498</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>17946</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4901272" y="2222481"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1592927</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>184130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>174736</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>22178</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4905510" y="2417213"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1586582</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>188362</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>168391</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>26410</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4899165" y="2611945"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3319</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2081</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>193795</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>30629</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4924569" y="3187664"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5420</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>173571</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>195896</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>11619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4926670" y="1644654"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>58395</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>35958</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>248871</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>43339</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3053478" y="872041"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>62633</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>29606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>253109</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>36987</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3057716" y="1077356"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>64747</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>31736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>255223</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>60284</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Picture 59"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3059830" y="2074319"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>68985</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>35980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>259461</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>64528</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 60"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3064068" y="1888063"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>73223</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>29641</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>263699</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>58189</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Picture 61"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3068306" y="1500724"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>77461</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>23302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>267937</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>30684</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="63" name="Picture 62"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3072544" y="1282719"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47819</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>25385</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238295</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>53933</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Picture 63"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3042902" y="2258468"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>52057</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>29617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>242533</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>58165</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="65" name="Picture 64"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3047140" y="2453200"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>73217</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19058</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>263693</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47606</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="Picture 67"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3068300" y="1680641"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5426</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4183</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>195902</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>32731</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="Picture 68"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4926676" y="3380266"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7557</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>6307</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>198033</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>24271</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="Picture 69"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4928807" y="3572890"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45592</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>12658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>236068</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>41206</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="Picture 70"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6840092" y="3388741"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>41520</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>29606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>231996</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>36987</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="Picture 71"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1332687" y="1077356"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>45758</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>23254</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>236234</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>30636</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="Picture 72"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1336925" y="1282671"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>45758</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>23268</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>236234</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>30649</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Picture 73"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1336925" y="859351"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>13760</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12707</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>204236</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>20089</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="Picture 74"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10459510" y="1272124"/>
           <a:ext cx="190476" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1924,11 +4086,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T45"/>
+  <dimension ref="B2:T44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H18" sqref="H18"/>
+      <selection pane="topRight" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,62 +4124,62 @@
     </row>
     <row r="3" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
-      <c r="C3" s="15">
+      <c r="C3" s="20">
         <v>40798</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16">
+      <c r="D3" s="20"/>
+      <c r="E3" s="21">
         <f>C3+7</f>
         <v>40805</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21">
         <f t="shared" ref="G3" si="0">E3+7</f>
         <v>40812</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="14">
+      <c r="H3" s="21"/>
+      <c r="I3" s="19">
         <f>G3+7</f>
         <v>40819</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14">
+      <c r="J3" s="19"/>
+      <c r="K3" s="19">
         <f>I3+7</f>
         <v>40826</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14">
+      <c r="L3" s="19"/>
+      <c r="M3" s="19">
         <f>K3+7</f>
         <v>40833</v>
       </c>
-      <c r="N3" s="14"/>
+      <c r="N3" s="19"/>
     </row>
     <row r="4" spans="2:20" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9"/>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="12" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="12" t="s">
+      <c r="F4" s="18"/>
+      <c r="G4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="12" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="12" t="s">
+      <c r="J4" s="18"/>
+      <c r="K4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="12" t="s">
+      <c r="L4" s="18"/>
+      <c r="M4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="13"/>
+      <c r="N4" s="18"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -2025,551 +4187,638 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="26" t="s">
+    <row r="5" spans="2:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" s="58"/>
-      <c r="J5" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="23"/>
-      <c r="N5" s="25" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="56"/>
+      <c r="F5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="57"/>
+      <c r="H5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="51"/>
+      <c r="J5" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="57"/>
+      <c r="L5" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" s="22"/>
+      <c r="N5" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:20" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="27"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="11" t="s">
-        <v>71</v>
+      <c r="B6" s="15"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="60"/>
+      <c r="F6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="58"/>
+      <c r="H6" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="I6" s="59"/>
-      <c r="J6" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="38"/>
-      <c r="N6" s="24" t="s">
+      <c r="J6" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="57"/>
+      <c r="L6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="54"/>
+      <c r="N6" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:20" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="39"/>
-      <c r="N7" s="28" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="57"/>
+      <c r="H7" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="51"/>
+      <c r="J7" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="57"/>
+      <c r="L7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="33"/>
+      <c r="N7" s="25" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="27"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" s="53"/>
-      <c r="J8" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="M8" s="31"/>
-      <c r="N8" s="32" t="s">
-        <v>16</v>
+      <c r="B8" s="15"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="62"/>
+      <c r="H8" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="64"/>
+      <c r="J8" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="62"/>
+      <c r="L8" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" s="28"/>
+      <c r="N8" s="53" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="I9" s="53"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="32"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="62"/>
+      <c r="H9" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="64"/>
+      <c r="J9" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="62"/>
+      <c r="L9" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="M9" s="54"/>
+      <c r="N9" s="55" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="27"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="I10" s="53"/>
-      <c r="J10" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="K10" s="34"/>
-      <c r="L10" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" s="32"/>
-      <c r="N10" s="33" t="s">
-        <v>20</v>
+      <c r="B10" s="15"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="64"/>
+      <c r="J10" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="62"/>
+      <c r="L10" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="54"/>
+      <c r="N10" s="55" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="27"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" s="53"/>
-      <c r="N11" s="56" t="s">
-        <v>21</v>
+      <c r="B11" s="15"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="65"/>
+      <c r="H11" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="62"/>
+      <c r="J11" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="K11" s="62"/>
+      <c r="L11" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" s="68"/>
+      <c r="N11" s="23" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="27"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="K12" s="30"/>
-      <c r="L12" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30" t="s">
-        <v>17</v>
+      <c r="B12" s="15"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="76" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="65"/>
+      <c r="H12" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="62"/>
+      <c r="J12" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="69"/>
+      <c r="L12" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="64"/>
+      <c r="N12" s="52" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="27"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="K13" s="30"/>
-      <c r="L13" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30" t="s">
-        <v>25</v>
+      <c r="B13" s="15"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="65"/>
+      <c r="H13" s="66" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" s="62"/>
+      <c r="J13" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="69"/>
+      <c r="L13" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13" s="69"/>
+      <c r="N13" s="70" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="27"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="66" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" s="34"/>
-      <c r="J14" s="40" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="71"/>
+      <c r="J14" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30" t="s">
-        <v>22</v>
+      <c r="K14" s="69"/>
+      <c r="L14" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" s="69"/>
+      <c r="N14" s="70" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="I15" s="36"/>
-      <c r="J15" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="42" t="s">
+      <c r="I15" s="71"/>
+      <c r="J15" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="73"/>
+      <c r="L15" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30" t="s">
-        <v>24</v>
+      <c r="M15" s="69"/>
+      <c r="N15" s="70" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="27"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="I16" s="36"/>
-      <c r="J16" s="43" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="36"/>
-      <c r="L16" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30" t="s">
-        <v>68</v>
+      <c r="I16" s="71"/>
+      <c r="J16" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" s="71"/>
+      <c r="L16" s="72" t="s">
+        <v>64</v>
+      </c>
+      <c r="M16" s="69"/>
+      <c r="N16" s="70" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="27"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="61"/>
+      <c r="J17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="71"/>
+      <c r="L17" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" s="69"/>
+      <c r="N17" s="70" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="73"/>
+      <c r="J18" s="74" t="s">
         <v>18</v>
       </c>
+      <c r="L18" s="35"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="74" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="18" spans="2:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="I18" s="8"/>
-      <c r="J18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N18" s="2" t="s">
+    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="16"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="39"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="77"/>
+      <c r="L19" s="78"/>
+      <c r="M19" s="89"/>
+      <c r="N19" s="50" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I19" s="29"/>
-      <c r="J19" s="42" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="B20" s="88"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="83"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="83"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="88"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="60"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="K21" s="10"/>
+    <row r="21" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="84" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="48"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="86"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="87"/>
+      <c r="N21" s="87"/>
     </row>
-    <row r="22" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="60"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="48"/>
+    <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="41"/>
+      <c r="G22" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="41"/>
+      <c r="I22" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" s="41"/>
+      <c r="K22" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="L22" s="41"/>
+      <c r="M22" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="N22" s="41"/>
     </row>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="H23" s="50"/>
-      <c r="I23" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="J23" s="50"/>
-      <c r="K23" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="L23" s="50"/>
-      <c r="M23" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="N23" s="50"/>
+      <c r="B23" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="41"/>
+      <c r="E23" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="41"/>
+      <c r="G23" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="41"/>
+      <c r="I23" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="41"/>
+      <c r="K23" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="L23" s="41"/>
+      <c r="M23" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="N23" s="41"/>
     </row>
     <row r="24" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="H24" s="50"/>
-      <c r="I24" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="J24" s="50"/>
-      <c r="K24" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="L24" s="50"/>
-      <c r="M24" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="N24" s="50"/>
+      <c r="B24" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="41"/>
+      <c r="E24" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="41"/>
+      <c r="G24" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="41"/>
+      <c r="I24" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="J24" s="41"/>
+      <c r="K24" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="L24" s="41"/>
+      <c r="M24" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="N24" s="41"/>
     </row>
     <row r="25" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="H25" s="50"/>
-      <c r="I25" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="J25" s="50"/>
-      <c r="K25" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="L25" s="50"/>
-      <c r="M25" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="N25" s="50"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="41"/>
+      <c r="G25" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="41"/>
+      <c r="I25" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="J25" s="41"/>
+      <c r="K25" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="L25" s="41"/>
+      <c r="M25" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="N25" s="41"/>
     </row>
     <row r="26" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="H26" s="50"/>
-      <c r="I26" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="50"/>
-      <c r="K26" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="L26" s="50"/>
-      <c r="M26" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="N26" s="50"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="41"/>
+      <c r="G26" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="41"/>
+      <c r="I26" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="J26" s="41"/>
+      <c r="K26" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="L26" s="41"/>
+      <c r="M26" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="N26" s="41"/>
     </row>
-    <row r="27" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27" s="50"/>
-      <c r="I27" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="J27" s="50"/>
-      <c r="K27" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="L27" s="50"/>
-      <c r="M27" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="N27" s="50"/>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C28" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="32"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C29" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="37"/>
+      <c r="C29" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="35" t="s">
-        <v>8</v>
+      <c r="D30" s="29" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="34" t="s">
-        <v>9</v>
+      <c r="D31" s="31" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C32" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="36" t="s">
-        <v>10</v>
+      <c r="C32" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>11</v>
+      <c r="C33" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="32" t="s">
-        <v>12</v>
+      <c r="D34" s="27" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>23</v>
+      <c r="C35" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="44" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" s="53" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="M22:N22"/>
     <mergeCell ref="M23:N23"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="M25:N25"/>
     <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="K22:L22"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="I22:J22"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G22:H22"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="B5:B17"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B5:B19"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="M4:N4"/>
@@ -2582,7 +4831,7 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
# Uploaded last iteration backlog, deliveryMap-GrupoLamas.pdf
</commit_message>
<xml_diff>
--- a/docs/deliveryMap-GrupoLamas.xlsx
+++ b/docs/deliveryMap-GrupoLamas.xlsx
@@ -894,6 +894,33 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -904,33 +931,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2475,14 +2475,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1605617</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>27188</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>175642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>187426</xdr:colOff>
+      <xdr:colOff>214640</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>13690</xdr:rowOff>
     </xdr:to>
@@ -2512,8 +2512,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4918200" y="2789725"/>
-          <a:ext cx="190476" cy="219048"/>
+          <a:off x="4939367" y="2760999"/>
+          <a:ext cx="187452" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2573,14 +2573,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1605617</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>27188</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>186249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>187426</xdr:colOff>
+      <xdr:colOff>214640</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>24297</xdr:rowOff>
     </xdr:to>
@@ -2610,8 +2610,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4918200" y="2038332"/>
-          <a:ext cx="190476" cy="219048"/>
+          <a:off x="4939367" y="2009606"/>
+          <a:ext cx="187452" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2623,13 +2623,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1188</xdr:colOff>
+      <xdr:colOff>14795</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>190493</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>191664</xdr:colOff>
+      <xdr:colOff>205271</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>28541</xdr:rowOff>
     </xdr:to>
@@ -2659,7 +2659,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4922438" y="1852076"/>
+          <a:off x="4926974" y="1823350"/>
           <a:ext cx="190476" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2672,13 +2672,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>5426</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>205320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>195902</xdr:colOff>
+      <xdr:colOff>32640</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5402</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>22202</xdr:rowOff>
     </xdr:to>
@@ -2708,8 +2708,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4926676" y="1464737"/>
-          <a:ext cx="190476" cy="219048"/>
+          <a:off x="4944819" y="1443570"/>
+          <a:ext cx="190476" cy="211489"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2769,14 +2769,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1588689</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>23867</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>179898</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>170498</xdr:colOff>
+      <xdr:colOff>211319</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>17946</xdr:rowOff>
     </xdr:to>
@@ -2806,26 +2806,26 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4901272" y="2222481"/>
-          <a:ext cx="190476" cy="219048"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1592927</xdr:colOff>
+          <a:off x="4936046" y="2193755"/>
+          <a:ext cx="187452" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>14498</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>184130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>174736</xdr:colOff>
+      <xdr:colOff>201950</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>22178</xdr:rowOff>
     </xdr:to>
@@ -2855,26 +2855,26 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4905510" y="2417213"/>
-          <a:ext cx="190476" cy="219048"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1586582</xdr:colOff>
+          <a:off x="4926677" y="2388487"/>
+          <a:ext cx="187452" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>21760</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>188362</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>168391</xdr:colOff>
+      <xdr:colOff>209212</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>26410</xdr:rowOff>
     </xdr:to>
@@ -2904,8 +2904,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4899165" y="2611945"/>
-          <a:ext cx="190476" cy="219048"/>
+          <a:off x="4933939" y="2583219"/>
+          <a:ext cx="187452" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2966,13 +2966,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>5420</xdr:colOff>
+      <xdr:colOff>32634</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>173571</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>195896</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5396</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>11619</xdr:rowOff>
     </xdr:to>
@@ -3002,7 +3002,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4926670" y="1644654"/>
+          <a:off x="4944813" y="1615928"/>
           <a:ext cx="190476" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4229,6 +4229,153 @@
         <a:xfrm>
           <a:off x="10497652" y="3384534"/>
           <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47366</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>237842</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>24902</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="83" name="Picture 82"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10484045" y="3547818"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9268</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12692</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>199744</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>41240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="84" name="Picture 83"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10445947" y="2788549"/>
+          <a:ext cx="190476" cy="219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>25598</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>206549</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>30368</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="85" name="Picture 84"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10462277" y="1634677"/>
+          <a:ext cx="180951" cy="219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4529,9 +4676,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P9" sqref="P9"/>
+      <selection pane="topRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4565,62 +4712,62 @@
     </row>
     <row r="3" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
-      <c r="C3" s="87">
+      <c r="C3" s="84">
         <v>40798</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="88">
+      <c r="D3" s="84"/>
+      <c r="E3" s="85">
         <f>C3+7</f>
         <v>40805</v>
       </c>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88">
+      <c r="F3" s="85"/>
+      <c r="G3" s="85">
         <f t="shared" ref="G3" si="0">E3+7</f>
         <v>40812</v>
       </c>
-      <c r="H3" s="88"/>
-      <c r="I3" s="86">
+      <c r="H3" s="85"/>
+      <c r="I3" s="83">
         <f>G3+7</f>
         <v>40819</v>
       </c>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86">
+      <c r="J3" s="83"/>
+      <c r="K3" s="83">
         <f>I3+7</f>
         <v>40826</v>
       </c>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86">
+      <c r="L3" s="83"/>
+      <c r="M3" s="83">
         <f>K3+7</f>
         <v>40833</v>
       </c>
-      <c r="N3" s="86"/>
+      <c r="N3" s="83"/>
     </row>
     <row r="4" spans="2:20" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="84" t="s">
+      <c r="D4" s="82"/>
+      <c r="E4" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="84" t="s">
+      <c r="F4" s="82"/>
+      <c r="G4" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="85"/>
-      <c r="I4" s="84" t="s">
+      <c r="H4" s="82"/>
+      <c r="I4" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="85"/>
-      <c r="K4" s="84" t="s">
+      <c r="J4" s="82"/>
+      <c r="K4" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="85"/>
-      <c r="M4" s="84" t="s">
+      <c r="L4" s="82"/>
+      <c r="M4" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="85"/>
+      <c r="N4" s="82"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -4629,7 +4776,7 @@
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="2:20" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="78" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="12"/>
@@ -4658,7 +4805,7 @@
       </c>
     </row>
     <row r="6" spans="2:20" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="82"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6" t="s">
         <v>100</v>
@@ -4685,7 +4832,7 @@
       </c>
     </row>
     <row r="7" spans="2:20" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="82"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6" t="s">
         <v>101</v>
@@ -4712,7 +4859,7 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="82"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="27"/>
       <c r="D8" s="37"/>
       <c r="E8" s="41"/>
@@ -4737,7 +4884,7 @@
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="82"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="27"/>
       <c r="D9" s="37"/>
       <c r="E9" s="44"/>
@@ -4762,7 +4909,7 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="82"/>
+      <c r="B10" s="79"/>
       <c r="C10" s="27"/>
       <c r="D10" s="37"/>
       <c r="E10" s="44"/>
@@ -4787,7 +4934,7 @@
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="82"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="27"/>
       <c r="D11" s="37"/>
       <c r="E11" s="21"/>
@@ -4812,7 +4959,7 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="82"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="27"/>
       <c r="D12" s="37"/>
       <c r="E12" s="62"/>
@@ -4837,7 +4984,7 @@
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="82"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="27"/>
       <c r="D13" s="37"/>
       <c r="E13" s="58"/>
@@ -4862,7 +5009,7 @@
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="82"/>
+      <c r="B14" s="79"/>
       <c r="C14" s="27"/>
       <c r="D14" s="37"/>
       <c r="E14" s="54"/>
@@ -4885,7 +5032,7 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="82"/>
+      <c r="B15" s="79"/>
       <c r="C15" s="27"/>
       <c r="D15" s="37"/>
       <c r="E15" s="54"/>
@@ -4908,7 +5055,7 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="82"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="27"/>
       <c r="D16" s="37"/>
       <c r="E16" s="54"/>
@@ -4931,7 +5078,7 @@
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="82"/>
+      <c r="B17" s="79"/>
       <c r="C17" s="27"/>
       <c r="D17" s="37"/>
       <c r="E17" s="54"/>
@@ -4954,7 +5101,7 @@
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="82"/>
+      <c r="B18" s="79"/>
       <c r="C18" s="27"/>
       <c r="D18" s="37"/>
       <c r="E18" s="54"/>
@@ -4974,7 +5121,7 @@
       </c>
     </row>
     <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="83"/>
+      <c r="B19" s="80"/>
       <c r="C19" s="69"/>
       <c r="D19" s="65"/>
       <c r="E19" s="64"/>
@@ -5026,146 +5173,146 @@
       <c r="B22" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="79"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="77" t="s">
+      <c r="C22" s="88"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="78"/>
-      <c r="G22" s="77" t="s">
+      <c r="F22" s="87"/>
+      <c r="G22" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="78"/>
-      <c r="I22" s="77" t="s">
+      <c r="H22" s="87"/>
+      <c r="I22" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="J22" s="78"/>
-      <c r="K22" s="77" t="s">
+      <c r="J22" s="87"/>
+      <c r="K22" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="78"/>
-      <c r="M22" s="77" t="s">
+      <c r="L22" s="87"/>
+      <c r="M22" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="N22" s="78"/>
+      <c r="N22" s="87"/>
     </row>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="77" t="s">
+      <c r="C23" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="78"/>
-      <c r="E23" s="77" t="s">
+      <c r="D23" s="87"/>
+      <c r="E23" s="86" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="78"/>
-      <c r="G23" s="77" t="s">
+      <c r="F23" s="87"/>
+      <c r="G23" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="H23" s="78"/>
-      <c r="I23" s="77" t="s">
+      <c r="H23" s="87"/>
+      <c r="I23" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="78"/>
-      <c r="K23" s="77" t="s">
+      <c r="J23" s="87"/>
+      <c r="K23" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="L23" s="78"/>
-      <c r="M23" s="77" t="s">
+      <c r="L23" s="87"/>
+      <c r="M23" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="N23" s="78"/>
+      <c r="N23" s="87"/>
     </row>
     <row r="24" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="77" t="s">
+      <c r="C24" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="78"/>
-      <c r="E24" s="77" t="s">
+      <c r="D24" s="87"/>
+      <c r="E24" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="78"/>
-      <c r="G24" s="77" t="s">
+      <c r="F24" s="87"/>
+      <c r="G24" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="H24" s="78"/>
-      <c r="I24" s="77" t="s">
+      <c r="H24" s="87"/>
+      <c r="I24" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="J24" s="78"/>
-      <c r="K24" s="77" t="s">
+      <c r="J24" s="87"/>
+      <c r="K24" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="78"/>
-      <c r="M24" s="77" t="s">
+      <c r="L24" s="87"/>
+      <c r="M24" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="N24" s="78"/>
+      <c r="N24" s="87"/>
     </row>
     <row r="25" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="77"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="77" t="s">
+      <c r="C25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="78"/>
-      <c r="G25" s="77" t="s">
+      <c r="F25" s="87"/>
+      <c r="G25" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="H25" s="78"/>
-      <c r="I25" s="77" t="s">
+      <c r="H25" s="87"/>
+      <c r="I25" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="J25" s="78"/>
-      <c r="K25" s="77" t="s">
+      <c r="J25" s="87"/>
+      <c r="K25" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="L25" s="78"/>
-      <c r="M25" s="77" t="s">
+      <c r="L25" s="87"/>
+      <c r="M25" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="78"/>
+      <c r="N25" s="87"/>
     </row>
     <row r="26" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="77" t="s">
+      <c r="C26" s="86"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="78"/>
-      <c r="G26" s="77" t="s">
+      <c r="F26" s="87"/>
+      <c r="G26" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="H26" s="78"/>
-      <c r="I26" s="77" t="s">
+      <c r="H26" s="87"/>
+      <c r="I26" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="J26" s="78"/>
-      <c r="K26" s="77" t="s">
+      <c r="J26" s="87"/>
+      <c r="K26" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="L26" s="78"/>
-      <c r="M26" s="77" t="s">
+      <c r="L26" s="87"/>
+      <c r="M26" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="N26" s="78"/>
+      <c r="N26" s="87"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C28" s="89" t="s">
+      <c r="C28" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="89"/>
+      <c r="D28" s="77"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C29" s="22" t="s">
@@ -5229,6 +5376,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="B5:B19"/>
     <mergeCell ref="K4:L4"/>
@@ -5245,42 +5420,34 @@
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxKeywordTaxHTField xmlns="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <TaxCatchAll xmlns="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100334BCE8D889DEF4D8118EAEBC7DDD6B2" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a9e8cdd0e52f65fd6658b59d8085902">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89803a6daf5a3c19d83a5939325ddd43" ns2:_="">
     <xsd:import namespace="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84"/>
@@ -5432,27 +5599,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B9CCC97-E7A1-4F27-9745-AD74F7374CAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxKeywordTaxHTField xmlns="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <TaxCatchAll xmlns="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D643F50-9742-4664-BEE4-3C5D7337C66D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5B402D4-7882-4319-AA0E-83388EE1282B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5468,28 +5639,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D643F50-9742-4664-BEE4-3C5D7337C66D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B9CCC97-E7A1-4F27-9745-AD74F7374CAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6805a2a6-1ebc-4cc8-9a06-34b4c1906a84"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>